<commit_message>
modified logic for modal display to verify examiner
</commit_message>
<xml_diff>
--- a/uploaded_files/exemption.xlsx
+++ b/uploaded_files/exemption.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4485FD5-3372-4749-90A4-EA812B51F865}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,190 +196,190 @@
     <t>Li Fang</t>
   </si>
   <si>
+    <t>Li Xiaoli</t>
+  </si>
+  <si>
+    <t>Li Yi</t>
+  </si>
+  <si>
+    <t>Lim Joo Hwee</t>
+  </si>
+  <si>
+    <t>Lin Feng</t>
+  </si>
+  <si>
+    <t>Lin Guosheng</t>
+  </si>
+  <si>
+    <t>Lin Shang-Wei</t>
+  </si>
+  <si>
+    <t>Lin Weisi</t>
+  </si>
+  <si>
+    <t>Liu Weichen</t>
+  </si>
+  <si>
+    <t>Liu Yang</t>
+  </si>
+  <si>
+    <t>Loke Yuan Ren</t>
+  </si>
+  <si>
+    <t>Long Cheng</t>
+  </si>
+  <si>
+    <t>Lu Shijian</t>
+  </si>
+  <si>
+    <t>Luo Jun</t>
+  </si>
+  <si>
+    <t>Mahardhika Pratama</t>
+  </si>
+  <si>
+    <t>Marius Erdt</t>
+  </si>
+  <si>
+    <t>Markus Schlapfer</t>
+  </si>
+  <si>
+    <t>Miao Chun Yan</t>
+  </si>
+  <si>
+    <t>Mohamed M. Sabry</t>
+  </si>
+  <si>
+    <t>Nadia Magnenat Thalmann</t>
+  </si>
+  <si>
+    <t>Ng Wee Keong</t>
+  </si>
+  <si>
+    <t>Oh Hong Lye</t>
+  </si>
+  <si>
+    <t>Ong Yew Soon</t>
+  </si>
+  <si>
+    <t>Owen Noel Newton Fernando</t>
+  </si>
+  <si>
+    <t>Pan, Sinno Jialin</t>
+  </si>
+  <si>
+    <t>Qian Kemao</t>
+  </si>
+  <si>
+    <t>Quek Hiok Chai</t>
+  </si>
+  <si>
+    <t>Rafael Enrique Banchs Martinez</t>
+  </si>
+  <si>
+    <t>Rajapakse Jagath Chandana</t>
+  </si>
+  <si>
+    <t>Rohan Mahadevan</t>
+  </si>
+  <si>
+    <t>Seah Hock Soon</t>
+  </si>
+  <si>
+    <t>Shar Lwin Khin</t>
+  </si>
+  <si>
+    <t>Shen Zhiqi</t>
+  </si>
+  <si>
+    <t>Smitha K G</t>
+  </si>
+  <si>
+    <t>Sourav Saha Bhowmick</t>
+  </si>
+  <si>
+    <t>Sourav Sen Gupta</t>
+  </si>
+  <si>
+    <t>Sun Aixin</t>
+  </si>
+  <si>
+    <t>Sun Chengzheng</t>
+  </si>
+  <si>
+    <t>Ta Nguyen Binh Duong</t>
+  </si>
+  <si>
+    <t>Tan Ah Hwee</t>
+  </si>
+  <si>
+    <t>Tan Kheng Leong</t>
+  </si>
+  <si>
+    <t>Tan Puay Siew</t>
+  </si>
+  <si>
+    <t>Tan Rui</t>
+  </si>
+  <si>
+    <t>Tang Xueyan</t>
+  </si>
+  <si>
+    <t>Thambipillai Srikanthan</t>
+  </si>
+  <si>
+    <t>Ulf Schlichtmann</t>
+  </si>
+  <si>
+    <t>Vijay Ramaseshan Chandrasekhar</t>
+  </si>
+  <si>
+    <t>Vun Chan Hua, Nicholas</t>
+  </si>
+  <si>
+    <t>Wen Yonggang</t>
+  </si>
+  <si>
+    <t>Xavier Bresson</t>
+  </si>
+  <si>
+    <t>Xiao Xiaokui</t>
+  </si>
+  <si>
+    <t>Xu Chi</t>
+  </si>
+  <si>
+    <t>Yeo Chai Kiat</t>
+  </si>
+  <si>
+    <t>Yu Han</t>
+  </si>
+  <si>
+    <t>Zhang Hanwang</t>
+  </si>
+  <si>
+    <t>Zhang Jie</t>
+  </si>
+  <si>
+    <t>Zhao Jun</t>
+  </si>
+  <si>
+    <t>Zheng Jianmin</t>
+  </si>
+  <si>
+    <t>Zinovi Rabinovich</t>
+  </si>
+  <si>
+    <t>Tay Kian Boon</t>
+  </si>
+  <si>
     <t>Li Mo</t>
-  </si>
-  <si>
-    <t>Li Xiaoli</t>
-  </si>
-  <si>
-    <t>Li Yi</t>
-  </si>
-  <si>
-    <t>Lim Joo Hwee</t>
-  </si>
-  <si>
-    <t>Lin Feng</t>
-  </si>
-  <si>
-    <t>Lin Guosheng</t>
-  </si>
-  <si>
-    <t>Lin Shang-Wei</t>
-  </si>
-  <si>
-    <t>Lin Weisi</t>
-  </si>
-  <si>
-    <t>Liu Weichen</t>
-  </si>
-  <si>
-    <t>Liu Yang</t>
-  </si>
-  <si>
-    <t>Loke Yuan Ren</t>
-  </si>
-  <si>
-    <t>Long Cheng</t>
-  </si>
-  <si>
-    <t>Lu Shijian</t>
-  </si>
-  <si>
-    <t>Luo Jun</t>
-  </si>
-  <si>
-    <t>Mahardhika Pratama</t>
-  </si>
-  <si>
-    <t>Marius Erdt</t>
-  </si>
-  <si>
-    <t>Markus Schlapfer</t>
-  </si>
-  <si>
-    <t>Miao Chun Yan</t>
-  </si>
-  <si>
-    <t>Mohamed M. Sabry</t>
-  </si>
-  <si>
-    <t>Nadia Magnenat Thalmann</t>
-  </si>
-  <si>
-    <t>Ng Wee Keong</t>
-  </si>
-  <si>
-    <t>Oh Hong Lye</t>
-  </si>
-  <si>
-    <t>Ong Yew Soon</t>
-  </si>
-  <si>
-    <t>Owen Noel Newton Fernando</t>
-  </si>
-  <si>
-    <t>Pan, Sinno Jialin</t>
-  </si>
-  <si>
-    <t>Qian Kemao</t>
-  </si>
-  <si>
-    <t>Quek Hiok Chai</t>
-  </si>
-  <si>
-    <t>Rafael Enrique Banchs Martinez</t>
-  </si>
-  <si>
-    <t>Rajapakse Jagath Chandana</t>
-  </si>
-  <si>
-    <t>Rohan Mahadevan</t>
-  </si>
-  <si>
-    <t>Seah Hock Soon</t>
-  </si>
-  <si>
-    <t>Shar Lwin Khin</t>
-  </si>
-  <si>
-    <t>Shen Zhiqi</t>
-  </si>
-  <si>
-    <t>Smitha K G</t>
-  </si>
-  <si>
-    <t>Sourav Saha Bhowmick</t>
-  </si>
-  <si>
-    <t>Sourav Sen Gupta</t>
-  </si>
-  <si>
-    <t>Sun Aixin</t>
-  </si>
-  <si>
-    <t>Sun Chengzheng</t>
-  </si>
-  <si>
-    <t>Ta Nguyen Binh Duong</t>
-  </si>
-  <si>
-    <t>Tan Ah Hwee</t>
-  </si>
-  <si>
-    <t>Tan Kheng Leong</t>
-  </si>
-  <si>
-    <t>Tan Puay Siew</t>
-  </si>
-  <si>
-    <t>Tan Rui</t>
-  </si>
-  <si>
-    <t>Tang Xueyan</t>
-  </si>
-  <si>
-    <t>Thambipillai Srikanthan</t>
-  </si>
-  <si>
-    <t>Ulf Schlichtmann</t>
-  </si>
-  <si>
-    <t>Vijay Ramaseshan Chandrasekhar</t>
-  </si>
-  <si>
-    <t>Vun Chan Hua, Nicholas</t>
-  </si>
-  <si>
-    <t>Wen Yonggang</t>
-  </si>
-  <si>
-    <t>Xavier Bresson</t>
-  </si>
-  <si>
-    <t>Xiao Xiaokui</t>
-  </si>
-  <si>
-    <t>Xu Chi</t>
-  </si>
-  <si>
-    <t>Yeo Chai Kiat</t>
-  </si>
-  <si>
-    <t>Yu Han</t>
-  </si>
-  <si>
-    <t>Zhang Hanwang</t>
-  </si>
-  <si>
-    <t>Zhang Jie</t>
-  </si>
-  <si>
-    <t>Zhao Jun</t>
-  </si>
-  <si>
-    <t>Zheng Jianmin</t>
-  </si>
-  <si>
-    <t>Zinovi Rabinovich</t>
-  </si>
-  <si>
-    <t>Tay Kian Boon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -773,20 +774,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="R109" sqref="R109"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -815,7 +816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -838,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -865,7 +866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -892,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -919,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -946,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -973,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1027,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1324,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1675,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1756,7 +1757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1810,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2001,7 +2002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2082,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2109,12 +2110,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="1">
@@ -2136,12 +2137,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="1">
@@ -2163,12 +2164,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="1">
@@ -2190,12 +2191,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="1">
@@ -2217,12 +2218,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="1">
@@ -2244,12 +2245,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="1">
@@ -2271,12 +2272,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="1">
@@ -2298,12 +2299,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="1">
@@ -2325,12 +2326,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="1">
@@ -2352,12 +2353,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="1">
@@ -2379,12 +2380,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="1">
@@ -2406,12 +2407,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="1">
@@ -2433,12 +2434,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="1">
@@ -2460,12 +2461,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="1">
@@ -2487,12 +2488,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="1">
@@ -2514,12 +2515,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="1">
@@ -2541,12 +2542,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="1">
@@ -2568,12 +2569,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="1">
@@ -2595,12 +2596,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="1">
@@ -2622,12 +2623,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="1">
@@ -2649,12 +2650,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="1">
@@ -2676,12 +2677,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="1">
@@ -2703,12 +2704,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="1">
@@ -2730,12 +2731,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="1">
@@ -2757,12 +2758,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="1">
@@ -2784,12 +2785,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="1">
@@ -2811,12 +2812,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="1">
@@ -2838,12 +2839,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="1">
@@ -2865,12 +2866,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="1">
@@ -2892,12 +2893,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="1">
@@ -2919,12 +2920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="1">
@@ -2946,12 +2947,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>48</v>
@@ -2975,12 +2976,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="1">
@@ -3002,12 +3003,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="1">
@@ -3029,12 +3030,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="1">
@@ -3056,12 +3057,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="1">
@@ -3083,12 +3084,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="1">
@@ -3110,12 +3111,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="1">
@@ -3137,12 +3138,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="1">
@@ -3164,12 +3165,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="1">
@@ -3191,12 +3192,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="1">
@@ -3218,12 +3219,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="1">
@@ -3245,12 +3246,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="1">
@@ -3272,12 +3273,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="1">
@@ -3299,12 +3300,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="1">
@@ -3326,12 +3327,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="1">
@@ -3353,12 +3354,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="1">
@@ -3380,12 +3381,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="1">
@@ -3407,12 +3408,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="1">
@@ -3434,12 +3435,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="1">
@@ -3461,12 +3462,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="1">
@@ -3488,12 +3489,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="1">
@@ -3515,12 +3516,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="1">
@@ -3542,12 +3543,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="1">
@@ -3569,12 +3570,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="1">
@@ -3596,12 +3597,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="1">
@@ -3623,12 +3624,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="1">
@@ -3650,12 +3651,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="1">
@@ -3677,12 +3678,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="1">
@@ -3704,12 +3705,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="1">

</xml_diff>